<commit_message>
Update TCs for Payment function
</commit_message>
<xml_diff>
--- a/Manual_Test_Cases_Zombie_Clothing_Store_Vinh_Tran.xlsx
+++ b/Manual_Test_Cases_Zombie_Clothing_Store_Vinh_Tran.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ECLIPSE-GIT\workspace\ZombieClothing_AUTE-IntelliJ-IDEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82521FF5-39FC-42F9-B420-F15523BE769E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4201713-AEC7-40FF-B54D-1042D6687A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{D5A25300-DCC6-4734-BB7F-F53EA33C6D7D}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" firstSheet="8" activeTab="11" xr2:uid="{D5A25300-DCC6-4734-BB7F-F53EA33C6D7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="16" r:id="rId1"/>
@@ -28,7 +28,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Func- &lt;&lt;Add to cart&gt;&gt;'!$A$22:$L$22</definedName>
@@ -1037,7 +1036,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="458">
   <si>
     <t>Func - Module</t>
   </si>
@@ -2006,28 +2005,13 @@
     <t>4. Input thiếu một trường thông tin bắt buộc</t>
   </si>
   <si>
-    <t>Kiểm tra rằng user thanh toán không thành công khi input thiếu một trường thông tin bắt buộc</t>
-  </si>
-  <si>
     <t>5. Quan sát thông báo lỗi từ website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống navigate user vào trang thanh toán sản phẩm
-- Hệ thống hiển thị thông báo lỗi ở cạnh trường bị thiếu!
-- Thanh toán không thành công!
-</t>
   </si>
   <si>
     <t>Kiểm tra rằng user thanh toán không thành công khi input thiếu nhiều hơn một trường thông tin bắt buộc</t>
   </si>
   <si>
     <t>4. Input thiếu từ hai trường thông tin bắt buộc trở lên</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống navigate user vào trang thanh toán sản phẩm
-- Hệ thống hiển thị thông báo lỗi ở cạnh các trường thông tin bị thiếu!
-- Thanh toán không thành công!
-</t>
   </si>
   <si>
     <t>Kiểm tra rằng user thanh toán không thành công khi input không hợp lệ vào các trường thông tin</t>
@@ -2719,6 +2703,28 @@
   <si>
     <t>Verify the website functions if they work properly automatically by designing Test scripts</t>
   </si>
+  <si>
+    <t>5. Input hợp lệ các trường còn lại</t>
+  </si>
+  <si>
+    <t>6. Quan sát thông báo lỗi từ website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống navigate user vào trang thanh toán sản phẩm
+- Hệ thống hiển thị thông báo lỗi tương ứng ở cạnh các trường thông tin bị thiếu!
+- Thanh toán không thành công!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra rằng user thanh toán 1 sản phẩm với số lượng 1 không thành công khi input thiếu một trường thông tin bắt buộc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống navigate user vào trang thanh toán sản phẩm
+- Hệ thống hiển thị giá tiền của sản phẩm với số lượng là 1
+- Hệ thống hiển thị thông báo lỗi tương ứng ở cạnh trường bị thiếu!
+- Thanh toán không thành công!
+</t>
+  </si>
 </sst>
 </file>
 
@@ -2934,7 +2940,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3022,6 +3028,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3364,7 +3376,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3886,6 +3898,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4254,13 +4269,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5844,38 +5859,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover Page"/>
-      <sheetName val="0. Project Information"/>
-      <sheetName val="1. Summary Report"/>
-      <sheetName val="2. Defects Report"/>
-      <sheetName val="Data Range"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="D2" t="str">
-            <v>Passed</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6178,7 +6161,7 @@
   </sheetPr>
   <dimension ref="B4:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
@@ -6191,20 +6174,20 @@
   <sheetData>
     <row r="4" spans="2:12" ht="42">
       <c r="D4" s="44" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="22.2">
       <c r="D6" s="45" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="20.399999999999999" customHeight="1">
       <c r="B10" s="47" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D10" s="70"/>
       <c r="E10" s="70"/>
@@ -6218,10 +6201,10 @@
     </row>
     <row r="11" spans="2:12" ht="20.399999999999999" customHeight="1">
       <c r="B11" s="47" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70"/>
@@ -6235,10 +6218,10 @@
     </row>
     <row r="12" spans="2:12" ht="20.399999999999999" customHeight="1">
       <c r="B12" s="47" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D12" s="70"/>
       <c r="E12" s="70"/>
@@ -6252,10 +6235,10 @@
     </row>
     <row r="13" spans="2:12" ht="54" customHeight="1">
       <c r="B13" s="46" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D13" s="71"/>
       <c r="E13" s="71"/>
@@ -6269,10 +6252,10 @@
     </row>
     <row r="14" spans="2:12" ht="20.399999999999999" customHeight="1">
       <c r="B14" s="47" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D14" s="70"/>
       <c r="E14" s="70"/>
@@ -6286,7 +6269,7 @@
     </row>
     <row r="15" spans="2:12" ht="20.399999999999999" customHeight="1">
       <c r="B15" s="47" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C15" s="70"/>
       <c r="D15" s="70"/>
@@ -6301,10 +6284,10 @@
     </row>
     <row r="16" spans="2:12" ht="20.399999999999999" customHeight="1">
       <c r="B16" s="47" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
@@ -6853,7 +6836,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="173" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H24" s="138" t="s">
         <v>28</v>
@@ -6973,7 +6956,7 @@
         <v>28</v>
       </c>
       <c r="G30" s="166" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H30" s="153" t="s">
         <v>28</v>
@@ -7155,7 +7138,7 @@
         <v>28</v>
       </c>
       <c r="G40" s="112" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H40" s="138" t="s">
         <v>28</v>
@@ -7291,7 +7274,7 @@
         <v>28</v>
       </c>
       <c r="G47" s="167" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H47" s="153" t="s">
         <v>28</v>
@@ -7473,7 +7456,7 @@
         <v>28</v>
       </c>
       <c r="G57" s="167" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H57" s="153" t="s">
         <v>28</v>
@@ -12085,8 +12068,8 @@
   </sheetPr>
   <dimension ref="A1:AU132"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -12600,7 +12583,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="167" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H24" s="138" t="s">
         <v>28</v>
@@ -12686,7 +12669,7 @@
         <v>28</v>
       </c>
       <c r="G28" s="167" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H28" s="153" t="s">
         <v>28</v>
@@ -12772,7 +12755,7 @@
         <v>28</v>
       </c>
       <c r="G32" s="167" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H32" s="138" t="s">
         <v>28</v>
@@ -12858,7 +12841,7 @@
         <v>28</v>
       </c>
       <c r="G36" s="167" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H36" s="153" t="s">
         <v>28</v>
@@ -12944,7 +12927,7 @@
         <v>28</v>
       </c>
       <c r="G40" s="167" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H40" s="153" t="s">
         <v>28</v>
@@ -13030,7 +13013,7 @@
         <v>28</v>
       </c>
       <c r="G44" s="167" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H44" s="153" t="s">
         <v>28</v>
@@ -17408,10 +17391,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AU115"/>
+  <dimension ref="A1:AU116"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -17621,7 +17604,7 @@
         <v>Build1</v>
       </c>
       <c r="B14" s="19">
-        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48442,B13)</f>
+        <f t="shared" ref="B14:G14" si="0">COUNTIF($L$23:$L$48443,B13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="19">
@@ -17656,7 +17639,7 @@
         <v>Build2</v>
       </c>
       <c r="B15" s="19">
-        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48442,B13)</f>
+        <f t="shared" ref="B15:G15" si="1">COUNTIF($K$23:$K$48443,B13)</f>
         <v>0</v>
       </c>
       <c r="C15" s="19">
@@ -17691,7 +17674,7 @@
         <v>Build3</v>
       </c>
       <c r="B16" s="19">
-        <f t="shared" ref="B16:G16" si="2">COUNTIF($J$23:$J$48442,B13)</f>
+        <f t="shared" ref="B16:G16" si="2">COUNTIF($J$23:$J$48443,B13)</f>
         <v>0</v>
       </c>
       <c r="C16" s="19">
@@ -17726,27 +17709,27 @@
         <v>Build4</v>
       </c>
       <c r="B17" s="19">
-        <f>COUNTIF($I$23:$I$48442,B13)</f>
+        <f>COUNTIF($I$23:$I$48443,B13)</f>
         <v>0</v>
       </c>
       <c r="C17" s="19">
-        <f>COUNTIF($I$23:$I$48442,C16)</f>
+        <f>COUNTIF($I$23:$I$48443,C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="19">
-        <f>COUNTIF($I$23:$I$48442,D13)</f>
+        <f>COUNTIF($I$23:$I$48443,D13)</f>
         <v>0</v>
       </c>
       <c r="E17" s="19">
-        <f>COUNTIF($I$23:$I$48442,E13)</f>
+        <f>COUNTIF($I$23:$I$48443,E13)</f>
         <v>0</v>
       </c>
       <c r="F17" s="19">
-        <f>COUNTIF($I$23:$I$48442,F13)</f>
+        <f>COUNTIF($I$23:$I$48443,F13)</f>
         <v>0</v>
       </c>
       <c r="G17" s="19">
-        <f>COUNTIF($I$23:$I$48442,G13)</f>
+        <f>COUNTIF($I$23:$I$48443,G13)</f>
         <v>0</v>
       </c>
       <c r="H17" s="20"/>
@@ -17761,8 +17744,8 @@
         <v>Build5</v>
       </c>
       <c r="B18" s="19">
-        <f t="shared" ref="B18:G18" si="3">COUNTIF($H$23:$H$48442,B13)</f>
-        <v>0</v>
+        <f t="shared" ref="B18:G18" si="3">COUNTIF($H$23:$H$48443,B13)</f>
+        <v>1</v>
       </c>
       <c r="C18" s="19">
         <f t="shared" si="3"/>
@@ -17774,7 +17757,7 @@
       </c>
       <c r="E18" s="19">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="19">
         <f t="shared" si="3"/>
@@ -17796,7 +17779,7 @@
       </c>
       <c r="B19" s="22">
         <f t="shared" ref="B19:G19" si="4">SUM(B14:B18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="22">
         <f t="shared" si="4"/>
@@ -17808,7 +17791,7 @@
       </c>
       <c r="E19" s="22">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" s="22">
         <f t="shared" si="4"/>
@@ -17909,7 +17892,7 @@
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
     </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="68.400000000000006" customHeight="1" outlineLevel="1">
       <c r="A24" s="145"/>
       <c r="B24" s="141" t="s">
         <v>164</v>
@@ -17925,7 +17908,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="167" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H24" s="153" t="s">
         <v>28</v>
@@ -18012,22 +17995,22 @@
         <v>85</v>
       </c>
       <c r="B29" s="135" t="s">
-        <v>259</v>
+        <v>456</v>
       </c>
       <c r="C29" s="136"/>
       <c r="D29" s="137"/>
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
-      <c r="H29" s="41" t="s">
-        <v>12</v>
+      <c r="H29" s="179" t="s">
+        <v>9</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
       <c r="K29" s="32"/>
       <c r="L29" s="32"/>
     </row>
-    <row r="30" spans="1:12" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
+    <row r="30" spans="1:12" s="28" customFormat="1" ht="60" customHeight="1" outlineLevel="1">
       <c r="A30" s="145"/>
       <c r="B30" s="141" t="s">
         <v>164</v>
@@ -18036,14 +18019,14 @@
         <v>229</v>
       </c>
       <c r="D30" s="146" t="s">
-        <v>261</v>
+        <v>457</v>
       </c>
       <c r="E30" s="172"/>
       <c r="F30" s="138" t="s">
         <v>28</v>
       </c>
       <c r="G30" s="167" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H30" s="153" t="s">
         <v>28</v>
@@ -18113,11 +18096,11 @@
       <c r="A34" s="145"/>
       <c r="B34" s="141"/>
       <c r="C34" s="27" t="s">
-        <v>260</v>
+        <v>453</v>
       </c>
       <c r="D34" s="146"/>
       <c r="E34" s="172"/>
-      <c r="F34" s="140"/>
+      <c r="F34" s="139"/>
       <c r="G34" s="167"/>
       <c r="H34" s="153"/>
       <c r="I34" s="153"/>
@@ -18125,81 +18108,81 @@
       <c r="K34" s="153"/>
       <c r="L34" s="153"/>
     </row>
-    <row r="35" spans="1:47" s="12" customFormat="1" ht="13.2">
-      <c r="A35" s="34" t="s">
+    <row r="35" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
+      <c r="A35" s="145"/>
+      <c r="B35" s="141"/>
+      <c r="C35" s="27" t="s">
+        <v>454</v>
+      </c>
+      <c r="D35" s="146"/>
+      <c r="E35" s="172"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="153"/>
+      <c r="I35" s="153"/>
+      <c r="J35" s="153"/>
+      <c r="K35" s="153"/>
+      <c r="L35" s="153"/>
+    </row>
+    <row r="36" spans="1:47" s="12" customFormat="1" ht="13.2">
+      <c r="A36" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="135" t="s">
-        <v>262</v>
-      </c>
-      <c r="C35" s="136"/>
-      <c r="D35" s="137"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="41" t="s">
+      <c r="B36" s="135" t="s">
+        <v>260</v>
+      </c>
+      <c r="C36" s="136"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-    </row>
-    <row r="36" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A36" s="145"/>
-      <c r="B36" s="141" t="s">
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+    </row>
+    <row r="37" spans="1:47" s="28" customFormat="1" ht="66.599999999999994" customHeight="1" outlineLevel="1">
+      <c r="A37" s="145"/>
+      <c r="B37" s="141" t="s">
         <v>164</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C37" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="D36" s="146" t="s">
-        <v>264</v>
-      </c>
-      <c r="E36" s="172"/>
-      <c r="F36" s="138" t="s">
+      <c r="D37" s="146" t="s">
+        <v>455</v>
+      </c>
+      <c r="E37" s="172"/>
+      <c r="F37" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="167" t="s">
-        <v>273</v>
-      </c>
-      <c r="H36" s="153" t="s">
+      <c r="G37" s="167" t="s">
+        <v>270</v>
+      </c>
+      <c r="H37" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="153" t="s">
+      <c r="I37" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="J36" s="153" t="s">
+      <c r="J37" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="153" t="s">
+      <c r="K37" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="L36" s="153" t="s">
+      <c r="L37" s="153" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A37" s="145"/>
-      <c r="B37" s="141"/>
-      <c r="C37" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="D37" s="146"/>
-      <c r="E37" s="172"/>
-      <c r="F37" s="139"/>
-      <c r="G37" s="167"/>
-      <c r="H37" s="153"/>
-      <c r="I37" s="153"/>
-      <c r="J37" s="153"/>
-      <c r="K37" s="153"/>
-      <c r="L37" s="153"/>
     </row>
     <row r="38" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
       <c r="A38" s="145"/>
       <c r="B38" s="141"/>
       <c r="C38" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D38" s="146"/>
       <c r="E38" s="172"/>
@@ -18215,7 +18198,7 @@
       <c r="A39" s="145"/>
       <c r="B39" s="141"/>
       <c r="C39" s="27" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="D39" s="146"/>
       <c r="E39" s="172"/>
@@ -18231,11 +18214,11 @@
       <c r="A40" s="145"/>
       <c r="B40" s="141"/>
       <c r="C40" s="27" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D40" s="146"/>
       <c r="E40" s="172"/>
-      <c r="F40" s="140"/>
+      <c r="F40" s="139"/>
       <c r="G40" s="167"/>
       <c r="H40" s="153"/>
       <c r="I40" s="153"/>
@@ -18243,81 +18226,81 @@
       <c r="K40" s="153"/>
       <c r="L40" s="153"/>
     </row>
-    <row r="41" spans="1:47" s="12" customFormat="1" ht="13.2">
-      <c r="A41" s="34" t="s">
+    <row r="41" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
+      <c r="A41" s="145"/>
+      <c r="B41" s="141"/>
+      <c r="C41" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="146"/>
+      <c r="E41" s="172"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="167"/>
+      <c r="H41" s="153"/>
+      <c r="I41" s="153"/>
+      <c r="J41" s="153"/>
+      <c r="K41" s="153"/>
+      <c r="L41" s="153"/>
+    </row>
+    <row r="42" spans="1:47" s="12" customFormat="1" ht="13.2">
+      <c r="A42" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="135" t="s">
-        <v>265</v>
-      </c>
-      <c r="C41" s="136"/>
-      <c r="D41" s="137"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="41" t="s">
+      <c r="B42" s="135" t="s">
+        <v>262</v>
+      </c>
+      <c r="C42" s="136"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-    </row>
-    <row r="42" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A42" s="145"/>
-      <c r="B42" s="141" t="s">
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+    </row>
+    <row r="43" spans="1:47" s="28" customFormat="1" ht="64.8" customHeight="1" outlineLevel="1">
+      <c r="A43" s="145"/>
+      <c r="B43" s="141" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="C43" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="D42" s="146" t="s">
-        <v>267</v>
-      </c>
-      <c r="E42" s="172"/>
-      <c r="F42" s="138" t="s">
+      <c r="D43" s="146" t="s">
+        <v>264</v>
+      </c>
+      <c r="E43" s="172"/>
+      <c r="F43" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="167" t="s">
-        <v>273</v>
-      </c>
-      <c r="H42" s="153" t="s">
+      <c r="G43" s="167" t="s">
+        <v>270</v>
+      </c>
+      <c r="H43" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="I42" s="153" t="s">
+      <c r="I43" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="J42" s="153" t="s">
+      <c r="J43" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="K42" s="153" t="s">
+      <c r="K43" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="L42" s="153" t="s">
+      <c r="L43" s="153" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="43" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
-      <c r="A43" s="145"/>
-      <c r="B43" s="141"/>
-      <c r="C43" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="D43" s="146"/>
-      <c r="E43" s="172"/>
-      <c r="F43" s="139"/>
-      <c r="G43" s="167"/>
-      <c r="H43" s="153"/>
-      <c r="I43" s="153"/>
-      <c r="J43" s="153"/>
-      <c r="K43" s="153"/>
-      <c r="L43" s="153"/>
     </row>
     <row r="44" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
       <c r="A44" s="145"/>
       <c r="B44" s="141"/>
       <c r="C44" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D44" s="146"/>
       <c r="E44" s="172"/>
@@ -18333,7 +18316,7 @@
       <c r="A45" s="145"/>
       <c r="B45" s="141"/>
       <c r="C45" s="27" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D45" s="146"/>
       <c r="E45" s="172"/>
@@ -18349,11 +18332,11 @@
       <c r="A46" s="145"/>
       <c r="B46" s="141"/>
       <c r="C46" s="27" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D46" s="146"/>
       <c r="E46" s="172"/>
-      <c r="F46" s="140"/>
+      <c r="F46" s="139"/>
       <c r="G46" s="167"/>
       <c r="H46" s="153"/>
       <c r="I46" s="153"/>
@@ -18361,54 +18344,21 @@
       <c r="K46" s="153"/>
       <c r="L46" s="153"/>
     </row>
-    <row r="47" spans="1:47">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
-      <c r="O47" s="29"/>
-      <c r="P47" s="29"/>
-      <c r="Q47" s="29"/>
-      <c r="R47" s="29"/>
-      <c r="S47" s="29"/>
-      <c r="T47" s="29"/>
-      <c r="U47" s="29"/>
-      <c r="V47" s="29"/>
-      <c r="W47" s="29"/>
-      <c r="X47" s="29"/>
-      <c r="Y47" s="29"/>
-      <c r="Z47" s="29"/>
-      <c r="AA47" s="29"/>
-      <c r="AB47" s="29"/>
-      <c r="AC47" s="29"/>
-      <c r="AD47" s="29"/>
-      <c r="AE47" s="29"/>
-      <c r="AF47" s="29"/>
-      <c r="AG47" s="29"/>
-      <c r="AH47" s="29"/>
-      <c r="AI47" s="29"/>
-      <c r="AJ47" s="29"/>
-      <c r="AK47" s="29"/>
-      <c r="AL47" s="29"/>
-      <c r="AM47" s="29"/>
-      <c r="AN47" s="29"/>
-      <c r="AO47" s="29"/>
-      <c r="AP47" s="29"/>
-      <c r="AQ47" s="29"/>
-      <c r="AR47" s="29"/>
-      <c r="AS47" s="29"/>
-      <c r="AT47" s="29"/>
-      <c r="AU47" s="29"/>
+    <row r="47" spans="1:47" s="28" customFormat="1" ht="47.4" customHeight="1" outlineLevel="1">
+      <c r="A47" s="145"/>
+      <c r="B47" s="141"/>
+      <c r="C47" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="D47" s="146"/>
+      <c r="E47" s="172"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="167"/>
+      <c r="H47" s="153"/>
+      <c r="I47" s="153"/>
+      <c r="J47" s="153"/>
+      <c r="K47" s="153"/>
+      <c r="L47" s="153"/>
     </row>
     <row r="48" spans="1:47">
       <c r="A48" s="29"/>
@@ -21742,6 +21692,55 @@
       <c r="AT115" s="29"/>
       <c r="AU115" s="29"/>
     </row>
+    <row r="116" spans="1:47">
+      <c r="A116" s="29"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
+      <c r="J116" s="29"/>
+      <c r="K116" s="29"/>
+      <c r="L116" s="29"/>
+      <c r="M116" s="29"/>
+      <c r="N116" s="29"/>
+      <c r="O116" s="29"/>
+      <c r="P116" s="29"/>
+      <c r="Q116" s="29"/>
+      <c r="R116" s="29"/>
+      <c r="S116" s="29"/>
+      <c r="T116" s="29"/>
+      <c r="U116" s="29"/>
+      <c r="V116" s="29"/>
+      <c r="W116" s="29"/>
+      <c r="X116" s="29"/>
+      <c r="Y116" s="29"/>
+      <c r="Z116" s="29"/>
+      <c r="AA116" s="29"/>
+      <c r="AB116" s="29"/>
+      <c r="AC116" s="29"/>
+      <c r="AD116" s="29"/>
+      <c r="AE116" s="29"/>
+      <c r="AF116" s="29"/>
+      <c r="AG116" s="29"/>
+      <c r="AH116" s="29"/>
+      <c r="AI116" s="29"/>
+      <c r="AJ116" s="29"/>
+      <c r="AK116" s="29"/>
+      <c r="AL116" s="29"/>
+      <c r="AM116" s="29"/>
+      <c r="AN116" s="29"/>
+      <c r="AO116" s="29"/>
+      <c r="AP116" s="29"/>
+      <c r="AQ116" s="29"/>
+      <c r="AR116" s="29"/>
+      <c r="AS116" s="29"/>
+      <c r="AT116" s="29"/>
+      <c r="AU116" s="29"/>
+    </row>
   </sheetData>
   <autoFilter ref="A22:L22" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="59">
@@ -21761,66 +21760,66 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="K30:K34"/>
-    <mergeCell ref="L30:L34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="H36:H40"/>
+    <mergeCell ref="K30:K35"/>
+    <mergeCell ref="L30:L35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="H37:H41"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="J36:J40"/>
-    <mergeCell ref="K36:K40"/>
-    <mergeCell ref="L36:L40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="G42:G46"/>
-    <mergeCell ref="H42:H46"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="E30:E34"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="J42:J46"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="K37:K41"/>
+    <mergeCell ref="L37:L41"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="F30:F35"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="H43:H47"/>
+    <mergeCell ref="I43:I47"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="D30:D35"/>
+    <mergeCell ref="E30:E35"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="J43:J47"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="F43:F47"/>
     <mergeCell ref="K24:K28"/>
     <mergeCell ref="L24:L28"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="I30:I34"/>
-    <mergeCell ref="J30:J34"/>
+    <mergeCell ref="G30:G35"/>
+    <mergeCell ref="H30:H35"/>
+    <mergeCell ref="I30:I35"/>
+    <mergeCell ref="J30:J35"/>
     <mergeCell ref="F24:F28"/>
     <mergeCell ref="G24:G28"/>
     <mergeCell ref="H24:H28"/>
     <mergeCell ref="I24:I28"/>
     <mergeCell ref="J24:J28"/>
-    <mergeCell ref="K42:K46"/>
-    <mergeCell ref="L42:L46"/>
+    <mergeCell ref="K43:K47"/>
+    <mergeCell ref="L43:L47"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H29:L29 H35:L35 H41:L41" xr:uid="{11027F35-BA24-4885-9DF2-21DEDD3FBA8B}">
+    <dataValidation type="list" allowBlank="1" sqref="H23:L23 H29:L29 H36:L36 H42:L42" xr:uid="{11027F35-BA24-4885-9DF2-21DEDD3FBA8B}">
       <formula1>$B$13:$G$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{1296A657-6786-4F76-9238-1D81241713A6}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="JE21:JG22 TA21:TC22 ACW21:ACY22 AMS21:AMU22 AWO21:AWQ22 BGK21:BGM22 BQG21:BQI22 CAC21:CAE22 CJY21:CKA22 CTU21:CTW22 DDQ21:DDS22 DNM21:DNO22 DXI21:DXK22 EHE21:EHG22 ERA21:ERC22 FAW21:FAY22 FKS21:FKU22 FUO21:FUQ22 GEK21:GEM22 GOG21:GOI22 GYC21:GYE22 HHY21:HIA22 HRU21:HRW22 IBQ21:IBS22 ILM21:ILO22 IVI21:IVK22 JFE21:JFG22 JPA21:JPC22 JYW21:JYY22 KIS21:KIU22 KSO21:KSQ22 LCK21:LCM22 LMG21:LMI22 LWC21:LWE22 MFY21:MGA22 MPU21:MPW22 MZQ21:MZS22 NJM21:NJO22 NTI21:NTK22 ODE21:ODG22 ONA21:ONC22 OWW21:OWY22 PGS21:PGU22 PQO21:PQQ22 QAK21:QAM22 QKG21:QKI22 QUC21:QUE22 RDY21:REA22 RNU21:RNW22 RXQ21:RXS22 SHM21:SHO22 SRI21:SRK22 TBE21:TBG22 TLA21:TLC22 TUW21:TUY22 UES21:UEU22 UOO21:UOQ22 UYK21:UYM22 VIG21:VII22 VSC21:VSE22 WBY21:WCA22 WLU21:WLW22 WVQ21:WVS22 H21 H22:L22" xr:uid="{2F104049-7000-489D-A4EB-8958D0966DB0}"/>
-    <dataValidation type="list" allowBlank="1" sqref="SHL23:SHO46 AWN23:AWQ46 MPT23:MPW46 BGJ23:BGM46 VIF23:VII46 BQF23:BQI46 MZP23:MZS46 CAB23:CAE46 SRH23:SRK46 CJX23:CKA46 NJL23:NJO46 CTT23:CTW46 WVP23:WVS46 DDP23:DDS46 NTH23:NTK46 DNL23:DNO46 TBD23:TBG46 DXH23:DXK46 ODD23:ODG46 EHD23:EHG46 VSB23:VSE46 EQZ23:ERC46 OMZ23:ONC46 FAV23:FAY46 TKZ23:TLC46 FKR23:FKU46 OWV23:OWY46 FUN23:FUQ46 JD23:JG46 GEJ23:GEM46 PGR23:PGU46 GOF23:GOI46 TUV23:TUY46 GYB23:GYE46 PQN23:PQQ46 HHX23:HIA46 WBX23:WCA46 HRT23:HRW46 QAJ23:QAM46 IBP23:IBS46 UER23:UEU46 ILL23:ILO46 QKF23:QKI46 IVH23:IVK46 SZ23:TC46 JFD23:JFG46 QUB23:QUE46 JOZ23:JPC46 UON23:UOQ46 JYV23:JYY46 RDX23:REA46 KIR23:KIU46 WLT23:WLW46 KSN23:KSQ46 RNT23:RNW46 LCJ23:LCM46 UYJ23:UYM46 LMF23:LMI46 RXP23:RXS46 LWB23:LWE46 ACV23:ACY46 MFX23:MGA46 AMR23:AMU46" xr:uid="{B07DEDAF-3B8E-4D71-B47F-53078ECC5E5D}">
+    <dataValidation type="list" allowBlank="1" sqref="SHL23:SHO47 AWN23:AWQ47 MPT23:MPW47 BGJ23:BGM47 VIF23:VII47 BQF23:BQI47 MZP23:MZS47 CAB23:CAE47 SRH23:SRK47 CJX23:CKA47 NJL23:NJO47 CTT23:CTW47 WVP23:WVS47 DDP23:DDS47 NTH23:NTK47 DNL23:DNO47 TBD23:TBG47 DXH23:DXK47 ODD23:ODG47 EHD23:EHG47 VSB23:VSE47 EQZ23:ERC47 OMZ23:ONC47 FAV23:FAY47 TKZ23:TLC47 FKR23:FKU47 OWV23:OWY47 FUN23:FUQ47 JD23:JG47 GEJ23:GEM47 PGR23:PGU47 GOF23:GOI47 TUV23:TUY47 GYB23:GYE47 PQN23:PQQ47 HHX23:HIA47 WBX23:WCA47 HRT23:HRW47 QAJ23:QAM47 IBP23:IBS47 UER23:UEU47 ILL23:ILO47 QKF23:QKI47 IVH23:IVK47 SZ23:TC47 JFD23:JFG47 QUB23:QUE47 JOZ23:JPC47 UON23:UOQ47 JYV23:JYY47 RDX23:REA47 KIR23:KIU47 WLT23:WLW47 KSN23:KSQ47 RNT23:RNW47 LCJ23:LCM47 UYJ23:UYM47 LMF23:LMI47 RXP23:RXS47 LWB23:LWE47 ACV23:ACY47 MFX23:MGA47 AMR23:AMU47" xr:uid="{B07DEDAF-3B8E-4D71-B47F-53078ECC5E5D}">
       <formula1>$A$14:$A$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A23 A29 A35 A41" numberStoredAsText="1"/>
+    <ignoredError sqref="A23 A29 A36 A42" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -21835,7 +21834,7 @@
   <dimension ref="B2:N278"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S78" sqref="S78"/>
+      <selection activeCell="C279" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -21850,7 +21849,7 @@
     <row r="2" spans="2:14" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="3" spans="2:14" ht="34.799999999999997" customHeight="1" thickBot="1">
       <c r="B3" s="87" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C3" s="87"/>
       <c r="D3" s="87"/>
@@ -21882,7 +21881,7 @@
     </row>
     <row r="5" spans="2:14" ht="15.75" customHeight="1">
       <c r="B5" s="101" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C5" s="101"/>
       <c r="D5" s="101"/>
@@ -21895,10 +21894,10 @@
     </row>
     <row r="6" spans="2:14" ht="35.4" customHeight="1">
       <c r="B6" s="55" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C6" s="88" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D6" s="88"/>
       <c r="E6" s="88"/>
@@ -21910,7 +21909,7 @@
     </row>
     <row r="7" spans="2:14" ht="21" customHeight="1" thickBot="1">
       <c r="B7" s="54" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C7" s="90">
         <v>1</v>
@@ -21936,7 +21935,7 @@
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1">
       <c r="B9" s="103" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C9" s="103"/>
       <c r="D9" s="103"/>
@@ -21949,7 +21948,7 @@
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1">
       <c r="B10" s="53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C10" s="92">
         <f>SUM(D21:D30)</f>
@@ -21965,7 +21964,7 @@
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1">
       <c r="B11" s="94" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C11" s="109" t="s">
         <v>9</v>
@@ -21975,7 +21974,7 @@
       <c r="F11" s="109"/>
       <c r="G11" s="92">
         <f>SUM(E21:E30)</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" s="92"/>
       <c r="I11" s="93"/>
@@ -21994,7 +21993,6 @@
       <c r="E12" s="96"/>
       <c r="F12" s="97"/>
       <c r="G12" s="98">
-        <f>'[2]Data Range'!E5</f>
         <v>0</v>
       </c>
       <c r="H12" s="99"/>
@@ -22011,7 +22009,7 @@
       </c>
       <c r="C13" s="105">
         <f>SUM(G21:G30)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="105"/>
       <c r="E13" s="105"/>
@@ -22030,7 +22028,6 @@
         <v>13</v>
       </c>
       <c r="C14" s="107">
-        <f>'[2]Data Range'!E7</f>
         <v>0</v>
       </c>
       <c r="D14" s="107"/>
@@ -22047,18 +22044,18 @@
     </row>
     <row r="15" spans="2:14" ht="15.75" customHeight="1">
       <c r="B15" s="72" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="51" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F15" s="50"/>
       <c r="G15" s="74" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H15" s="75"/>
       <c r="I15" s="49"/>
@@ -22071,7 +22068,7 @@
     <row r="16" spans="2:14" ht="33.6" customHeight="1" thickBot="1">
       <c r="B16" s="73"/>
       <c r="C16" s="76" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D16" s="77"/>
       <c r="E16" s="77"/>
@@ -22105,29 +22102,29 @@
     </row>
     <row r="18" spans="2:14" ht="15.75" customHeight="1">
       <c r="B18" s="82" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C18" s="82" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D18" s="82" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E18" s="85" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F18" s="85"/>
       <c r="G18" s="85"/>
       <c r="H18" s="85"/>
       <c r="I18" s="86"/>
       <c r="J18" s="110" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="K18" s="85"/>
       <c r="L18" s="85"/>
       <c r="M18" s="86"/>
       <c r="N18" s="82" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="15.75" customHeight="1">
@@ -22135,25 +22132,25 @@
       <c r="C19" s="83"/>
       <c r="D19" s="83"/>
       <c r="E19" s="85" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F19" s="85"/>
       <c r="G19" s="85"/>
       <c r="H19" s="86"/>
       <c r="I19" s="82" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J19" s="111" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="K19" s="111" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="L19" s="82" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="M19" s="82" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="N19" s="83"/>
     </row>
@@ -22185,7 +22182,7 @@
         <v>119</v>
       </c>
       <c r="C21" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D21" s="61">
         <v>10</v>
@@ -22220,7 +22217,7 @@
         <v>118</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D22" s="61">
         <v>2</v>
@@ -22255,7 +22252,7 @@
         <v>77</v>
       </c>
       <c r="C23" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D23" s="61">
         <v>15</v>
@@ -22290,7 +22287,7 @@
         <v>162</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D24" s="61">
         <v>4</v>
@@ -22325,7 +22322,7 @@
         <v>173</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D25" s="61">
         <v>16</v>
@@ -22357,10 +22354,10 @@
     </row>
     <row r="26" spans="2:14" ht="36" customHeight="1">
       <c r="B26" s="61" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D26" s="61">
         <v>13</v>
@@ -22395,7 +22392,7 @@
         <v>192</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D27" s="61">
         <v>3</v>
@@ -22430,7 +22427,7 @@
         <v>177</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D28" s="61">
         <v>5</v>
@@ -22465,7 +22462,7 @@
         <v>224</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D29" s="61">
         <v>6</v>
@@ -22500,19 +22497,19 @@
         <v>251</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D30" s="61">
         <v>4</v>
       </c>
       <c r="E30" s="61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="61">
         <v>0</v>
       </c>
       <c r="G30" s="61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H30" s="61">
         <v>0</v>
@@ -22535,7 +22532,7 @@
         <v>9</v>
       </c>
       <c r="C276" s="56">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="277" spans="2:3" ht="15.75" customHeight="1">
@@ -22551,7 +22548,7 @@
         <v>12</v>
       </c>
       <c r="C278" s="56">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -23114,7 +23111,7 @@
       </c>
       <c r="F24" s="153"/>
       <c r="G24" s="154" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H24" s="148"/>
       <c r="I24" s="138"/>
@@ -23190,7 +23187,7 @@
       </c>
       <c r="F28" s="138"/>
       <c r="G28" s="112" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H28" s="142"/>
       <c r="I28" s="138"/>
@@ -23284,7 +23281,7 @@
         <v>28</v>
       </c>
       <c r="G33" s="112" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H33" s="115" t="s">
         <v>28</v>
@@ -23388,7 +23385,7 @@
         <v>28</v>
       </c>
       <c r="G38" s="112" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H38" s="115" t="s">
         <v>28</v>
@@ -23492,7 +23489,7 @@
         <v>28</v>
       </c>
       <c r="G43" s="112" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H43" s="115" t="s">
         <v>28</v>
@@ -23596,7 +23593,7 @@
         <v>28</v>
       </c>
       <c r="G48" s="112" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H48" s="115" t="s">
         <v>28</v>
@@ -23700,7 +23697,7 @@
         <v>28</v>
       </c>
       <c r="G53" s="112" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H53" s="115" t="s">
         <v>28</v>
@@ -23804,7 +23801,7 @@
         <v>28</v>
       </c>
       <c r="G58" s="112" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H58" s="115" t="s">
         <v>28</v>
@@ -23908,7 +23905,7 @@
         <v>28</v>
       </c>
       <c r="G63" s="112" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H63" s="115" t="s">
         <v>28</v>
@@ -24012,7 +24009,7 @@
         <v>28</v>
       </c>
       <c r="G68" s="112" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H68" s="115" t="s">
         <v>28</v>
@@ -33136,7 +33133,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="112" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H24" s="115" t="s">
         <v>28</v>
@@ -33270,7 +33267,7 @@
         <v>28</v>
       </c>
       <c r="G31" s="161" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H31" s="118" t="s">
         <v>28</v>
@@ -42332,7 +42329,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="166" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H24" s="138" t="s">
         <v>28</v>
@@ -42498,7 +42495,7 @@
       </c>
       <c r="F33" s="138"/>
       <c r="G33" s="112" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H33" s="142"/>
       <c r="I33" s="138"/>
@@ -42590,7 +42587,7 @@
       </c>
       <c r="F38" s="138"/>
       <c r="G38" s="112" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H38" s="142"/>
       <c r="I38" s="138"/>
@@ -42682,7 +42679,7 @@
       </c>
       <c r="F43" s="138"/>
       <c r="G43" s="112" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H43" s="142"/>
       <c r="I43" s="138"/>
@@ -42774,7 +42771,7 @@
       </c>
       <c r="F48" s="138"/>
       <c r="G48" s="112" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H48" s="142"/>
       <c r="I48" s="138"/>
@@ -42866,7 +42863,7 @@
       </c>
       <c r="F53" s="138"/>
       <c r="G53" s="112" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H53" s="142"/>
       <c r="I53" s="138"/>
@@ -42958,7 +42955,7 @@
       </c>
       <c r="F58" s="138"/>
       <c r="G58" s="112" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H58" s="142"/>
       <c r="I58" s="138"/>
@@ -43050,7 +43047,7 @@
       </c>
       <c r="F63" s="138"/>
       <c r="G63" s="112" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H63" s="142"/>
       <c r="I63" s="138"/>
@@ -43142,7 +43139,7 @@
       </c>
       <c r="F68" s="138"/>
       <c r="G68" s="112" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H68" s="142"/>
       <c r="I68" s="138"/>
@@ -43218,7 +43215,7 @@
       </c>
       <c r="F72" s="153"/>
       <c r="G72" s="166" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H72" s="168"/>
       <c r="I72" s="153"/>
@@ -43278,7 +43275,7 @@
       </c>
       <c r="F75" s="138"/>
       <c r="G75" s="112" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H75" s="142"/>
       <c r="I75" s="138"/>
@@ -43370,7 +43367,7 @@
       </c>
       <c r="F80" s="138"/>
       <c r="G80" s="112" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H80" s="142"/>
       <c r="I80" s="138"/>
@@ -43462,7 +43459,7 @@
       </c>
       <c r="F85" s="138"/>
       <c r="G85" s="112" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H85" s="142"/>
       <c r="I85" s="138"/>
@@ -43554,7 +43551,7 @@
       </c>
       <c r="F90" s="138"/>
       <c r="G90" s="112" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H90" s="142"/>
       <c r="I90" s="138"/>
@@ -43646,7 +43643,7 @@
       </c>
       <c r="F95" s="138"/>
       <c r="G95" s="112" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H95" s="142"/>
       <c r="I95" s="138"/>
@@ -45983,7 +45980,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="166" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H24" s="138" t="s">
         <v>28</v>
@@ -46071,7 +46068,7 @@
         <v>28</v>
       </c>
       <c r="G28" s="166" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H28" s="153" t="s">
         <v>28</v>
@@ -46175,7 +46172,7 @@
         <v>28</v>
       </c>
       <c r="G33" s="166" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H33" s="153" t="s">
         <v>28</v>
@@ -46246,7 +46243,7 @@
         <v>87</v>
       </c>
       <c r="B37" s="135" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C37" s="136"/>
       <c r="D37" s="137"/>
@@ -46279,7 +46276,7 @@
         <v>28</v>
       </c>
       <c r="G38" s="166" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H38" s="153" t="s">
         <v>28</v>
@@ -52458,7 +52455,7 @@
         <v>84</v>
       </c>
       <c r="B23" s="135" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C23" s="136"/>
       <c r="D23" s="137"/>
@@ -52482,7 +52479,7 @@
         <v>163</v>
       </c>
       <c r="D24" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E24" s="153" t="s">
         <v>28</v>
@@ -52491,7 +52488,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H24" s="153" t="s">
         <v>28</v>
@@ -52513,7 +52510,7 @@
       <c r="A25" s="145"/>
       <c r="B25" s="141"/>
       <c r="C25" s="27" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D25" s="146"/>
       <c r="E25" s="153"/>
@@ -52546,7 +52543,7 @@
         <v>85</v>
       </c>
       <c r="B27" s="135" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C27" s="136"/>
       <c r="D27" s="137"/>
@@ -52570,7 +52567,7 @@
         <v>163</v>
       </c>
       <c r="D28" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E28" s="153" t="s">
         <v>28</v>
@@ -52579,7 +52576,7 @@
         <v>28</v>
       </c>
       <c r="G28" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H28" s="153" t="s">
         <v>28</v>
@@ -52601,7 +52598,7 @@
       <c r="A29" s="145"/>
       <c r="B29" s="141"/>
       <c r="C29" s="27" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D29" s="146"/>
       <c r="E29" s="153"/>
@@ -52634,7 +52631,7 @@
         <v>86</v>
       </c>
       <c r="B31" s="135" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C31" s="136"/>
       <c r="D31" s="137"/>
@@ -52658,7 +52655,7 @@
         <v>163</v>
       </c>
       <c r="D32" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E32" s="153" t="s">
         <v>28</v>
@@ -52667,7 +52664,7 @@
         <v>28</v>
       </c>
       <c r="G32" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H32" s="153" t="s">
         <v>28</v>
@@ -52689,7 +52686,7 @@
       <c r="A33" s="145"/>
       <c r="B33" s="141"/>
       <c r="C33" s="27" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D33" s="146"/>
       <c r="E33" s="153"/>
@@ -52722,7 +52719,7 @@
         <v>87</v>
       </c>
       <c r="B35" s="135" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C35" s="136"/>
       <c r="D35" s="137"/>
@@ -52746,7 +52743,7 @@
         <v>163</v>
       </c>
       <c r="D36" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E36" s="153" t="s">
         <v>28</v>
@@ -52755,7 +52752,7 @@
         <v>28</v>
       </c>
       <c r="G36" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H36" s="153" t="s">
         <v>28</v>
@@ -52777,7 +52774,7 @@
       <c r="A37" s="145"/>
       <c r="B37" s="141"/>
       <c r="C37" s="27" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D37" s="146"/>
       <c r="E37" s="153"/>
@@ -52810,7 +52807,7 @@
         <v>88</v>
       </c>
       <c r="B39" s="135" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C39" s="136"/>
       <c r="D39" s="137"/>
@@ -52834,7 +52831,7 @@
         <v>163</v>
       </c>
       <c r="D40" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E40" s="153" t="s">
         <v>28</v>
@@ -52843,7 +52840,7 @@
         <v>28</v>
       </c>
       <c r="G40" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H40" s="153" t="s">
         <v>28</v>
@@ -52865,7 +52862,7 @@
       <c r="A41" s="145"/>
       <c r="B41" s="141"/>
       <c r="C41" s="27" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D41" s="146"/>
       <c r="E41" s="153"/>
@@ -52898,7 +52895,7 @@
         <v>89</v>
       </c>
       <c r="B43" s="135" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C43" s="136"/>
       <c r="D43" s="137"/>
@@ -52922,7 +52919,7 @@
         <v>163</v>
       </c>
       <c r="D44" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E44" s="153" t="s">
         <v>28</v>
@@ -52931,7 +52928,7 @@
         <v>28</v>
       </c>
       <c r="G44" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H44" s="153" t="s">
         <v>28</v>
@@ -52953,7 +52950,7 @@
       <c r="A45" s="145"/>
       <c r="B45" s="141"/>
       <c r="C45" s="27" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D45" s="146"/>
       <c r="E45" s="153"/>
@@ -52986,7 +52983,7 @@
         <v>90</v>
       </c>
       <c r="B47" s="135" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C47" s="136"/>
       <c r="D47" s="137"/>
@@ -53010,7 +53007,7 @@
         <v>163</v>
       </c>
       <c r="D48" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E48" s="153" t="s">
         <v>28</v>
@@ -53019,7 +53016,7 @@
         <v>28</v>
       </c>
       <c r="G48" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H48" s="153" t="s">
         <v>28</v>
@@ -53041,7 +53038,7 @@
       <c r="A49" s="145"/>
       <c r="B49" s="141"/>
       <c r="C49" s="27" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D49" s="146"/>
       <c r="E49" s="153"/>
@@ -53074,7 +53071,7 @@
         <v>91</v>
       </c>
       <c r="B51" s="135" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C51" s="136"/>
       <c r="D51" s="137"/>
@@ -53098,7 +53095,7 @@
         <v>163</v>
       </c>
       <c r="D52" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E52" s="153" t="s">
         <v>28</v>
@@ -53107,7 +53104,7 @@
         <v>28</v>
       </c>
       <c r="G52" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H52" s="153" t="s">
         <v>28</v>
@@ -53129,7 +53126,7 @@
       <c r="A53" s="145"/>
       <c r="B53" s="141"/>
       <c r="C53" s="27" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D53" s="146"/>
       <c r="E53" s="153"/>
@@ -53162,7 +53159,7 @@
         <v>92</v>
       </c>
       <c r="B55" s="135" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C55" s="136"/>
       <c r="D55" s="137"/>
@@ -53186,7 +53183,7 @@
         <v>163</v>
       </c>
       <c r="D56" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E56" s="153" t="s">
         <v>28</v>
@@ -53195,7 +53192,7 @@
         <v>28</v>
       </c>
       <c r="G56" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H56" s="153" t="s">
         <v>28</v>
@@ -53217,7 +53214,7 @@
       <c r="A57" s="145"/>
       <c r="B57" s="141"/>
       <c r="C57" s="27" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D57" s="146"/>
       <c r="E57" s="153"/>
@@ -53250,7 +53247,7 @@
         <v>93</v>
       </c>
       <c r="B59" s="135" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C59" s="136"/>
       <c r="D59" s="137"/>
@@ -53274,7 +53271,7 @@
         <v>163</v>
       </c>
       <c r="D60" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E60" s="153" t="s">
         <v>28</v>
@@ -53283,7 +53280,7 @@
         <v>28</v>
       </c>
       <c r="G60" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H60" s="153" t="s">
         <v>28</v>
@@ -53305,7 +53302,7 @@
       <c r="A61" s="145"/>
       <c r="B61" s="141"/>
       <c r="C61" s="27" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D61" s="146"/>
       <c r="E61" s="153"/>
@@ -53338,7 +53335,7 @@
         <v>138</v>
       </c>
       <c r="B63" s="135" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C63" s="136"/>
       <c r="D63" s="137"/>
@@ -53362,7 +53359,7 @@
         <v>163</v>
       </c>
       <c r="D64" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E64" s="153" t="s">
         <v>28</v>
@@ -53371,7 +53368,7 @@
         <v>28</v>
       </c>
       <c r="G64" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H64" s="153" t="s">
         <v>28</v>
@@ -53393,7 +53390,7 @@
       <c r="A65" s="145"/>
       <c r="B65" s="141"/>
       <c r="C65" s="27" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D65" s="146"/>
       <c r="E65" s="153"/>
@@ -53426,7 +53423,7 @@
         <v>144</v>
       </c>
       <c r="B67" s="135" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C67" s="136"/>
       <c r="D67" s="137"/>
@@ -53450,7 +53447,7 @@
         <v>163</v>
       </c>
       <c r="D68" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E68" s="153" t="s">
         <v>28</v>
@@ -53459,7 +53456,7 @@
         <v>28</v>
       </c>
       <c r="G68" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H68" s="153" t="s">
         <v>28</v>
@@ -53481,7 +53478,7 @@
       <c r="A69" s="145"/>
       <c r="B69" s="141"/>
       <c r="C69" s="27" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D69" s="146"/>
       <c r="E69" s="153"/>
@@ -53514,7 +53511,7 @@
         <v>147</v>
       </c>
       <c r="B71" s="135" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C71" s="136"/>
       <c r="D71" s="137"/>
@@ -53538,7 +53535,7 @@
         <v>163</v>
       </c>
       <c r="D72" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E72" s="153" t="s">
         <v>28</v>
@@ -53547,7 +53544,7 @@
         <v>28</v>
       </c>
       <c r="G72" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H72" s="153" t="s">
         <v>28</v>
@@ -53569,7 +53566,7 @@
       <c r="A73" s="145"/>
       <c r="B73" s="141"/>
       <c r="C73" s="27" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D73" s="146"/>
       <c r="E73" s="153"/>
@@ -53602,7 +53599,7 @@
         <v>151</v>
       </c>
       <c r="B75" s="135" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C75" s="136"/>
       <c r="D75" s="137"/>
@@ -53626,7 +53623,7 @@
         <v>163</v>
       </c>
       <c r="D76" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E76" s="153" t="s">
         <v>28</v>
@@ -53635,7 +53632,7 @@
         <v>28</v>
       </c>
       <c r="G76" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H76" s="153" t="s">
         <v>28</v>
@@ -53657,7 +53654,7 @@
       <c r="A77" s="145"/>
       <c r="B77" s="141"/>
       <c r="C77" s="27" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D77" s="146"/>
       <c r="E77" s="153"/>
@@ -53690,7 +53687,7 @@
         <v>156</v>
       </c>
       <c r="B79" s="135" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C79" s="136"/>
       <c r="D79" s="137"/>
@@ -53714,7 +53711,7 @@
         <v>163</v>
       </c>
       <c r="D80" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E80" s="153" t="s">
         <v>28</v>
@@ -53723,7 +53720,7 @@
         <v>28</v>
       </c>
       <c r="G80" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H80" s="153" t="s">
         <v>28</v>
@@ -53745,7 +53742,7 @@
       <c r="A81" s="145"/>
       <c r="B81" s="141"/>
       <c r="C81" s="27" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D81" s="146"/>
       <c r="E81" s="153"/>
@@ -53775,10 +53772,10 @@
     </row>
     <row r="83" spans="1:47" s="12" customFormat="1" ht="13.2">
       <c r="A83" s="34" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B83" s="135" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C83" s="136"/>
       <c r="D83" s="137"/>
@@ -53802,7 +53799,7 @@
         <v>163</v>
       </c>
       <c r="D84" s="146" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E84" s="153" t="s">
         <v>28</v>
@@ -53811,7 +53808,7 @@
         <v>28</v>
       </c>
       <c r="G84" s="169" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H84" s="153" t="s">
         <v>28</v>
@@ -53833,7 +53830,7 @@
       <c r="A85" s="145"/>
       <c r="B85" s="141"/>
       <c r="C85" s="27" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D85" s="146"/>
       <c r="E85" s="153"/>
@@ -56558,7 +56555,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="160" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C5" s="160"/>
       <c r="D5" s="160"/>
@@ -56982,7 +56979,7 @@
         <v>84</v>
       </c>
       <c r="B23" s="135" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C23" s="136"/>
       <c r="D23" s="137"/>
@@ -57006,7 +57003,7 @@
         <v>163</v>
       </c>
       <c r="D24" s="146" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E24" s="153" t="s">
         <v>28</v>
@@ -57015,7 +57012,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="169" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="H24" s="153" t="s">
         <v>28</v>
@@ -57037,7 +57034,7 @@
       <c r="A25" s="145"/>
       <c r="B25" s="141"/>
       <c r="C25" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D25" s="146"/>
       <c r="E25" s="153"/>
@@ -57053,7 +57050,7 @@
       <c r="A26" s="145"/>
       <c r="B26" s="141"/>
       <c r="C26" s="27" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D26" s="146"/>
       <c r="E26" s="153"/>
@@ -57069,7 +57066,7 @@
       <c r="A27" s="145"/>
       <c r="B27" s="141"/>
       <c r="C27" s="27" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D27" s="146"/>
       <c r="E27" s="153"/>
@@ -57086,7 +57083,7 @@
         <v>85</v>
       </c>
       <c r="B28" s="135" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C28" s="136"/>
       <c r="D28" s="137"/>
@@ -57110,7 +57107,7 @@
         <v>163</v>
       </c>
       <c r="D29" s="146" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E29" s="153" t="s">
         <v>28</v>
@@ -57119,7 +57116,7 @@
         <v>28</v>
       </c>
       <c r="G29" s="169" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H29" s="153" t="s">
         <v>28</v>
@@ -57141,7 +57138,7 @@
       <c r="A30" s="145"/>
       <c r="B30" s="141"/>
       <c r="C30" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D30" s="146"/>
       <c r="E30" s="153"/>
@@ -57157,7 +57154,7 @@
       <c r="A31" s="145"/>
       <c r="B31" s="141"/>
       <c r="C31" s="38" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D31" s="146"/>
       <c r="E31" s="153"/>
@@ -57173,7 +57170,7 @@
       <c r="A32" s="145"/>
       <c r="B32" s="141"/>
       <c r="C32" s="27" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D32" s="146"/>
       <c r="E32" s="153"/>
@@ -57189,7 +57186,7 @@
       <c r="A33" s="145"/>
       <c r="B33" s="141"/>
       <c r="C33" s="27" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D33" s="146"/>
       <c r="E33" s="153"/>
@@ -57206,7 +57203,7 @@
         <v>86</v>
       </c>
       <c r="B34" s="135" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C34" s="136"/>
       <c r="D34" s="137"/>
@@ -57230,7 +57227,7 @@
         <v>163</v>
       </c>
       <c r="D35" s="146" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="E35" s="153" t="s">
         <v>28</v>
@@ -57239,7 +57236,7 @@
         <v>28</v>
       </c>
       <c r="G35" s="169" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H35" s="153" t="s">
         <v>28</v>
@@ -57261,7 +57258,7 @@
       <c r="A36" s="145"/>
       <c r="B36" s="141"/>
       <c r="C36" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D36" s="146"/>
       <c r="E36" s="153"/>
@@ -57277,7 +57274,7 @@
       <c r="A37" s="145"/>
       <c r="B37" s="141"/>
       <c r="C37" s="38" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D37" s="146"/>
       <c r="E37" s="153"/>
@@ -57293,7 +57290,7 @@
       <c r="A38" s="145"/>
       <c r="B38" s="141"/>
       <c r="C38" s="27" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D38" s="146"/>
       <c r="E38" s="153"/>
@@ -57309,7 +57306,7 @@
       <c r="A39" s="145"/>
       <c r="B39" s="141"/>
       <c r="C39" s="27" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D39" s="146"/>
       <c r="E39" s="153"/>
@@ -57326,7 +57323,7 @@
         <v>87</v>
       </c>
       <c r="B40" s="135" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C40" s="136"/>
       <c r="D40" s="137"/>
@@ -57350,7 +57347,7 @@
         <v>163</v>
       </c>
       <c r="D41" s="146" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E41" s="153" t="s">
         <v>28</v>
@@ -57359,7 +57356,7 @@
         <v>28</v>
       </c>
       <c r="G41" s="169" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H41" s="153" t="s">
         <v>28</v>
@@ -57381,7 +57378,7 @@
       <c r="A42" s="145"/>
       <c r="B42" s="141"/>
       <c r="C42" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D42" s="146"/>
       <c r="E42" s="153"/>
@@ -57397,7 +57394,7 @@
       <c r="A43" s="145"/>
       <c r="B43" s="141"/>
       <c r="C43" s="38" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D43" s="146"/>
       <c r="E43" s="153"/>
@@ -57413,7 +57410,7 @@
       <c r="A44" s="145"/>
       <c r="B44" s="141"/>
       <c r="C44" s="27" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D44" s="146"/>
       <c r="E44" s="153"/>
@@ -57429,7 +57426,7 @@
       <c r="A45" s="145"/>
       <c r="B45" s="141"/>
       <c r="C45" s="27" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D45" s="146"/>
       <c r="E45" s="153"/>
@@ -57446,7 +57443,7 @@
         <v>88</v>
       </c>
       <c r="B46" s="135" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C46" s="136"/>
       <c r="D46" s="137"/>
@@ -57470,7 +57467,7 @@
         <v>163</v>
       </c>
       <c r="D47" s="146" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E47" s="153" t="s">
         <v>28</v>
@@ -57479,7 +57476,7 @@
         <v>28</v>
       </c>
       <c r="G47" s="169" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H47" s="153" t="s">
         <v>28</v>
@@ -57501,7 +57498,7 @@
       <c r="A48" s="145"/>
       <c r="B48" s="141"/>
       <c r="C48" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D48" s="146"/>
       <c r="E48" s="153"/>
@@ -57517,7 +57514,7 @@
       <c r="A49" s="145"/>
       <c r="B49" s="141"/>
       <c r="C49" s="38" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D49" s="146"/>
       <c r="E49" s="153"/>
@@ -57533,7 +57530,7 @@
       <c r="A50" s="145"/>
       <c r="B50" s="141"/>
       <c r="C50" s="27" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D50" s="146"/>
       <c r="E50" s="153"/>
@@ -57550,7 +57547,7 @@
         <v>89</v>
       </c>
       <c r="B51" s="135" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C51" s="136"/>
       <c r="D51" s="137"/>
@@ -57574,7 +57571,7 @@
         <v>163</v>
       </c>
       <c r="D52" s="146" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E52" s="153" t="s">
         <v>28</v>
@@ -57583,7 +57580,7 @@
         <v>28</v>
       </c>
       <c r="G52" s="169" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H52" s="153" t="s">
         <v>28</v>
@@ -57605,7 +57602,7 @@
       <c r="A53" s="145"/>
       <c r="B53" s="141"/>
       <c r="C53" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D53" s="146"/>
       <c r="E53" s="153"/>
@@ -57621,7 +57618,7 @@
       <c r="A54" s="145"/>
       <c r="B54" s="141"/>
       <c r="C54" s="38" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D54" s="146"/>
       <c r="E54" s="153"/>
@@ -57637,7 +57634,7 @@
       <c r="A55" s="145"/>
       <c r="B55" s="141"/>
       <c r="C55" s="27" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D55" s="146"/>
       <c r="E55" s="153"/>
@@ -57653,7 +57650,7 @@
       <c r="A56" s="145"/>
       <c r="B56" s="141"/>
       <c r="C56" s="27" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D56" s="146"/>
       <c r="E56" s="153"/>
@@ -57670,7 +57667,7 @@
         <v>90</v>
       </c>
       <c r="B57" s="135" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C57" s="136"/>
       <c r="D57" s="137"/>
@@ -57694,7 +57691,7 @@
         <v>163</v>
       </c>
       <c r="D58" s="146" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E58" s="153" t="s">
         <v>28</v>
@@ -57703,7 +57700,7 @@
         <v>28</v>
       </c>
       <c r="G58" s="169" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H58" s="153" t="s">
         <v>28</v>
@@ -57725,7 +57722,7 @@
       <c r="A59" s="145"/>
       <c r="B59" s="141"/>
       <c r="C59" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D59" s="146"/>
       <c r="E59" s="153"/>
@@ -57741,7 +57738,7 @@
       <c r="A60" s="145"/>
       <c r="B60" s="141"/>
       <c r="C60" s="38" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D60" s="146"/>
       <c r="E60" s="153"/>
@@ -57757,7 +57754,7 @@
       <c r="A61" s="145"/>
       <c r="B61" s="141"/>
       <c r="C61" s="27" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D61" s="146"/>
       <c r="E61" s="153"/>
@@ -57773,7 +57770,7 @@
       <c r="A62" s="145"/>
       <c r="B62" s="141"/>
       <c r="C62" s="27" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D62" s="146"/>
       <c r="E62" s="153"/>
@@ -57790,7 +57787,7 @@
         <v>91</v>
       </c>
       <c r="B63" s="135" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C63" s="136"/>
       <c r="D63" s="137"/>
@@ -57814,7 +57811,7 @@
         <v>163</v>
       </c>
       <c r="D64" s="146" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E64" s="153" t="s">
         <v>28</v>
@@ -57823,7 +57820,7 @@
         <v>28</v>
       </c>
       <c r="G64" s="169" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H64" s="153" t="s">
         <v>28</v>
@@ -57845,7 +57842,7 @@
       <c r="A65" s="145"/>
       <c r="B65" s="141"/>
       <c r="C65" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D65" s="146"/>
       <c r="E65" s="153"/>
@@ -57861,7 +57858,7 @@
       <c r="A66" s="145"/>
       <c r="B66" s="141"/>
       <c r="C66" s="27" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D66" s="146"/>
       <c r="E66" s="153"/>
@@ -57877,7 +57874,7 @@
       <c r="A67" s="145"/>
       <c r="B67" s="141"/>
       <c r="C67" s="27" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D67" s="146"/>
       <c r="E67" s="153"/>
@@ -57894,7 +57891,7 @@
         <v>92</v>
       </c>
       <c r="B68" s="135" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C68" s="136"/>
       <c r="D68" s="137"/>
@@ -57918,7 +57915,7 @@
         <v>163</v>
       </c>
       <c r="D69" s="146" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E69" s="153" t="s">
         <v>28</v>
@@ -57927,7 +57924,7 @@
         <v>28</v>
       </c>
       <c r="G69" s="169" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H69" s="153" t="s">
         <v>28</v>
@@ -57949,7 +57946,7 @@
       <c r="A70" s="145"/>
       <c r="B70" s="141"/>
       <c r="C70" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D70" s="146"/>
       <c r="E70" s="153"/>
@@ -57965,7 +57962,7 @@
       <c r="A71" s="145"/>
       <c r="B71" s="141"/>
       <c r="C71" s="27" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D71" s="146"/>
       <c r="E71" s="153"/>
@@ -57981,7 +57978,7 @@
       <c r="A72" s="145"/>
       <c r="B72" s="141"/>
       <c r="C72" s="27" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D72" s="146"/>
       <c r="E72" s="153"/>
@@ -57998,7 +57995,7 @@
         <v>93</v>
       </c>
       <c r="B73" s="135" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C73" s="136"/>
       <c r="D73" s="137"/>
@@ -58022,7 +58019,7 @@
         <v>163</v>
       </c>
       <c r="D74" s="146" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E74" s="153" t="s">
         <v>28</v>
@@ -58031,7 +58028,7 @@
         <v>28</v>
       </c>
       <c r="G74" s="169" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H74" s="153" t="s">
         <v>28</v>
@@ -58053,7 +58050,7 @@
       <c r="A75" s="145"/>
       <c r="B75" s="141"/>
       <c r="C75" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D75" s="146"/>
       <c r="E75" s="153"/>
@@ -58069,7 +58066,7 @@
       <c r="A76" s="145"/>
       <c r="B76" s="141"/>
       <c r="C76" s="38" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D76" s="146"/>
       <c r="E76" s="153"/>
@@ -58085,7 +58082,7 @@
       <c r="A77" s="145"/>
       <c r="B77" s="141"/>
       <c r="C77" s="27" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D77" s="146"/>
       <c r="E77" s="153"/>
@@ -58101,7 +58098,7 @@
       <c r="A78" s="145"/>
       <c r="B78" s="141"/>
       <c r="C78" s="27" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D78" s="146"/>
       <c r="E78" s="153"/>
@@ -58118,7 +58115,7 @@
         <v>138</v>
       </c>
       <c r="B79" s="135" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C79" s="136"/>
       <c r="D79" s="137"/>
@@ -58142,7 +58139,7 @@
         <v>163</v>
       </c>
       <c r="D80" s="146" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E80" s="153" t="s">
         <v>28</v>
@@ -58151,7 +58148,7 @@
         <v>28</v>
       </c>
       <c r="G80" s="169" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="H80" s="153" t="s">
         <v>28</v>
@@ -58173,7 +58170,7 @@
       <c r="A81" s="145"/>
       <c r="B81" s="141"/>
       <c r="C81" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D81" s="146"/>
       <c r="E81" s="153"/>
@@ -58189,7 +58186,7 @@
       <c r="A82" s="145"/>
       <c r="B82" s="141"/>
       <c r="C82" s="38" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D82" s="146"/>
       <c r="E82" s="153"/>
@@ -58205,7 +58202,7 @@
       <c r="A83" s="145"/>
       <c r="B83" s="141"/>
       <c r="C83" s="27" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D83" s="146"/>
       <c r="E83" s="153"/>
@@ -58221,7 +58218,7 @@
       <c r="A84" s="145"/>
       <c r="B84" s="141"/>
       <c r="C84" s="27" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D84" s="146"/>
       <c r="E84" s="153"/>
@@ -58238,7 +58235,7 @@
         <v>144</v>
       </c>
       <c r="B85" s="135" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C85" s="136"/>
       <c r="D85" s="137"/>
@@ -58262,7 +58259,7 @@
         <v>163</v>
       </c>
       <c r="D86" s="146" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E86" s="153" t="s">
         <v>28</v>
@@ -58271,7 +58268,7 @@
         <v>28</v>
       </c>
       <c r="G86" s="169" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H86" s="153" t="s">
         <v>28</v>
@@ -58293,7 +58290,7 @@
       <c r="A87" s="145"/>
       <c r="B87" s="141"/>
       <c r="C87" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D87" s="146"/>
       <c r="E87" s="153"/>
@@ -58309,7 +58306,7 @@
       <c r="A88" s="145"/>
       <c r="B88" s="141"/>
       <c r="C88" s="38" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D88" s="146"/>
       <c r="E88" s="153"/>
@@ -58325,7 +58322,7 @@
       <c r="A89" s="145"/>
       <c r="B89" s="141"/>
       <c r="C89" s="27" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D89" s="146"/>
       <c r="E89" s="153"/>
@@ -58341,7 +58338,7 @@
       <c r="A90" s="145"/>
       <c r="B90" s="141"/>
       <c r="C90" s="27" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D90" s="146"/>
       <c r="E90" s="153"/>
@@ -58358,7 +58355,7 @@
         <v>147</v>
       </c>
       <c r="B91" s="135" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C91" s="136"/>
       <c r="D91" s="137"/>
@@ -58382,7 +58379,7 @@
         <v>163</v>
       </c>
       <c r="D92" s="146" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E92" s="153" t="s">
         <v>28</v>
@@ -58391,7 +58388,7 @@
         <v>28</v>
       </c>
       <c r="G92" s="169" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H92" s="153" t="s">
         <v>28</v>
@@ -58413,7 +58410,7 @@
       <c r="A93" s="145"/>
       <c r="B93" s="141"/>
       <c r="C93" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D93" s="146"/>
       <c r="E93" s="153"/>
@@ -58429,7 +58426,7 @@
       <c r="A94" s="145"/>
       <c r="B94" s="141"/>
       <c r="C94" s="38" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D94" s="146"/>
       <c r="E94" s="153"/>
@@ -58445,7 +58442,7 @@
       <c r="A95" s="145"/>
       <c r="B95" s="141"/>
       <c r="C95" s="27" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D95" s="146"/>
       <c r="E95" s="153"/>
@@ -58461,7 +58458,7 @@
       <c r="A96" s="145"/>
       <c r="B96" s="141"/>
       <c r="C96" s="27" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D96" s="146"/>
       <c r="E96" s="153"/>
@@ -59190,7 +59187,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="166" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H24" s="153" t="s">
         <v>28</v>
@@ -59278,7 +59275,7 @@
         <v>28</v>
       </c>
       <c r="G28" s="166" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H28" s="153" t="s">
         <v>28</v>
@@ -59366,7 +59363,7 @@
         <v>28</v>
       </c>
       <c r="G32" s="166" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H32" s="153" t="s">
         <v>28</v>

</xml_diff>